<commit_message>
Update Entrenamiento Regresión Lineal.xlsx
</commit_message>
<xml_diff>
--- a/Apuntes y otros/Entrenamiento Regresión Lineal.xlsx
+++ b/Apuntes y otros/Entrenamiento Regresión Lineal.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhYNkWBvQCkURLYQJ7ShiLJ5PXBiA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjqO5PzMOECkLSF1tHtEhrdbAAwIQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -46,12 +46,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,21 +66,65 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -299,70 +344,75 @@
     <col customWidth="1" min="1" max="1" width="10.71"/>
     <col customWidth="1" min="2" max="2" width="17.29"/>
     <col customWidth="1" min="3" max="3" width="10.57"/>
-    <col customWidth="1" min="4" max="26" width="10.71"/>
+    <col customWidth="1" min="4" max="4" width="10.71"/>
+    <col customWidth="1" min="5" max="5" width="23.71"/>
+    <col customWidth="1" min="6" max="6" width="10.57"/>
+    <col customWidth="1" min="7" max="26" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>0.660189096324695</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <v>0.712529932199559</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>0.651436848279831</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>0.642567248009633</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>0.675043374477354</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>0.699567585927725</v>
       </c>
     </row>
@@ -1337,30 +1387,6 @@
     <row r="974" ht="14.25" customHeight="1"/>
     <row r="975" ht="14.25" customHeight="1"/>
     <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>

</xml_diff>